<commit_message>
New model Sept 21
</commit_message>
<xml_diff>
--- a/assets/points.xlsx
+++ b/assets/points.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B2125813-FDA8-4906-A5A9-130D3ED52EA9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E001106C-3BE8-4C26-B722-99A8B760A982}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>time_given</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>hard, es6, functions</t>
+  </si>
+  <si>
+    <t>dom</t>
+  </si>
+  <si>
+    <t>dom-interview</t>
   </si>
 </sst>
 </file>
@@ -516,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P26" si="1">O3*5</f>
+        <f t="shared" ref="P3:P28" si="1">O3*5</f>
         <v>5</v>
       </c>
     </row>
@@ -849,16 +855,11 @@
         <f>((E8/C8)+(D8/F8)) * H8</f>
         <v>240</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="4">
-        <v>5</v>
-      </c>
-      <c r="P8" s="4">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8"/>
+      <c r="P8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -891,14 +892,7 @@
         <v>240</v>
       </c>
       <c r="N9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O9">
-        <v>10</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -931,15 +925,15 @@
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
-      <c r="N10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="1"/>
-        <v>20</v>
+      <c r="N10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="4">
+        <v>5</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -972,15 +966,15 @@
         <f>((E11/C11)+(D11/F11)) * H11</f>
         <v>60</v>
       </c>
-      <c r="N11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O11" s="4">
-        <v>4</v>
-      </c>
-      <c r="P11" s="4">
-        <f t="shared" si="1"/>
-        <v>20</v>
+      <c r="N11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1014,14 +1008,14 @@
         <v>140</v>
       </c>
       <c r="N12" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="O12">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="P12">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1054,15 +1048,15 @@
         <f t="shared" si="0"/>
         <v>256.66666666666669</v>
       </c>
-      <c r="N13" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13">
-        <v>3</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="1"/>
-        <v>15</v>
+      <c r="N13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="4">
+        <v>4</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -1095,14 +1089,14 @@
         <v>1.9090909090909092</v>
       </c>
       <c r="N14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O14">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="P14">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1116,14 +1110,14 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="N15" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P15">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -1137,19 +1131,19 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="N16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P16">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -1161,114 +1155,138 @@
     </row>
     <row r="18" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N18" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="O18">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="P18">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N19" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P19">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N20" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="O20">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="P20">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N21" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="O21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P21">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N22" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="O22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P22">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P23">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N24" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="O24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P24">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="O25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P25">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
         <v>6</v>
       </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="N2:O26">
+  <sortState ref="N2:O28">
     <sortCondition ref="N1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>